<commit_message>
Fix color of Dakota graph
</commit_message>
<xml_diff>
--- a/pa-28-236/pa-28-236.xlsx
+++ b/pa-28-236/pa-28-236.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-28-236/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{594ECDE4-B920-CC45-B960-242F87C33A5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D313454-206C-5D4F-A195-D32D044194FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="780" windowWidth="28160" windowHeight="15360" activeTab="1" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
+    <workbookView xWindow="320" yWindow="780" windowWidth="28160" windowHeight="15360" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
   </bookViews>
   <sheets>
     <sheet name="KIAS Vs. % Power (50F ROP)" sheetId="1" r:id="rId1"/>
@@ -386,11 +386,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2244,7 +2244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147924CF-2EF1-8C42-B7BB-87C12FB00719}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2313,6 +2313,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -2321,7 +2322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49353E1-1EC1-5A40-9077-1E137B7BE37E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Make note for wheel fairing difference and adjust axis
</commit_message>
<xml_diff>
--- a/pa-28-236/pa-28-236.xlsx
+++ b/pa-28-236/pa-28-236.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-28-236/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D313454-206C-5D4F-A195-D32D044194FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBEE3F4-F832-3948-A757-E17D6D20AF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="780" windowWidth="28160" windowHeight="15360" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
+    <workbookView xWindow="320" yWindow="780" windowWidth="28160" windowHeight="15660" activeTab="1" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
   </bookViews>
   <sheets>
     <sheet name="KIAS Vs. % Power (50F ROP)" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
               <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>, No Wheel Fairings, Sea Level, 59</a:t>
+              <a:t>, Sea Level, 59</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1100" b="1" i="0">
@@ -505,19 +505,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>139.12</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125.96</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>118.44</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.97999999999999</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.759999999999991</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -614,7 +614,7 @@
         <c:crossAx val="948993503"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.1"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
         <c:minorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:valAx>
@@ -691,7 +691,7 @@
         <c:crossAx val="951141263"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="5"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:spPr>
@@ -736,6 +736,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -838,7 +839,7 @@
               <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Peak EGT, No Wheel Fairings, Sea Level, 59</a:t>
+              <a:t>Peak EGT, Sea Level, 59</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1100" b="1" i="0">
@@ -1030,13 +1031,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>116.55999999999999</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.1</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1133,14 +1134,14 @@
         <c:crossAx val="948993503"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.1"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
         <c:minorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="948993503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="140"/>
+          <c:max val="135"/>
           <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1210,7 +1211,7 @@
         <c:crossAx val="951141263"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="5"/>
         <c:minorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
@@ -1233,6 +1234,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -1836,6 +1838,133 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.67898</cdr:x>
+      <cdr:y>0.80351</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91026</cdr:x>
+      <cdr:y>0.91491</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D5D7C72-9350-104F-AA91-E81935A111EA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4323360" y="3786851"/>
+          <a:ext cx="1472676" cy="524982"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:rPr>
+            <a:t>Note: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:rPr>
+            <a:t>Subtract Approx. 6% If Wheel Fairings Are Not Installed</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1876,6 +2005,69 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.70555</cdr:x>
+      <cdr:y>0.79077</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93722</cdr:x>
+      <cdr:y>0.90802</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B289706-9784-ED4F-A8E0-BFD5877AA209}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4492543" y="3639255"/>
+          <a:ext cx="1475124" cy="539635"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:rPr>
+            <a:t>Note: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:rPr>
+            <a:t>Subtract Approx. 6% If Wheel Fairings Are Not Installed</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2244,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147924CF-2EF1-8C42-B7BB-87C12FB00719}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2268,8 +2460,8 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>148*0.94</f>
-        <v>139.12</v>
+        <f>148</f>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2277,8 +2469,8 @@
         <v>0.85</v>
       </c>
       <c r="B3">
-        <f>134*0.94</f>
-        <v>125.96</v>
+        <f>134</f>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2286,8 +2478,8 @@
         <v>0.75</v>
       </c>
       <c r="B4">
-        <f>126*0.94</f>
-        <v>118.44</v>
+        <f>126</f>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2295,8 +2487,8 @@
         <v>0.65</v>
       </c>
       <c r="B5">
-        <f>117*0.94</f>
-        <v>109.97999999999999</v>
+        <f>117</f>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2304,8 +2496,8 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B6">
-        <f>104*0.94</f>
-        <v>97.759999999999991</v>
+        <f>104</f>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2322,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49353E1-1EC1-5A40-9077-1E137B7BE37E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2346,8 +2538,8 @@
         <v>0.75</v>
       </c>
       <c r="B2">
-        <f>124*0.94</f>
-        <v>116.55999999999999</v>
+        <f>124</f>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2355,8 +2547,8 @@
         <v>0.65</v>
       </c>
       <c r="B3">
-        <f>115*0.94</f>
-        <v>108.1</v>
+        <f>115</f>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2364,8 +2556,8 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B4">
-        <f>100*0.94</f>
-        <v>94</v>
+        <f>100</f>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add rough tradeoffs between fuel flow, speed, and range
</commit_message>
<xml_diff>
--- a/pa-28-236/pa-28-236.xlsx
+++ b/pa-28-236/pa-28-236.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-28-236/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D134248-5C8D-3D47-AC9D-B6BC3FF3D664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D6E4D2-9F6E-FE41-8D24-57B0EF22A6E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="780" windowWidth="37760" windowHeight="19340" activeTab="1" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
+    <workbookView xWindow="7200" yWindow="3060" windowWidth="37760" windowHeight="19340" activeTab="3" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
   </bookViews>
   <sheets>
     <sheet name="KIAS Vs. % Power (50F ROP)" sheetId="1" r:id="rId1"/>
     <sheet name="KIAS Vs. % Power (Peak EGT)" sheetId="3" r:id="rId2"/>
     <sheet name="Altitude Vs. IAS at 65% (Eco)" sheetId="4" r:id="rId3"/>
+    <sheet name="Fuel Flow Comparison" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Percent Power</t>
   </si>
@@ -53,6 +54,24 @@
   </si>
   <si>
     <t>KTAS</t>
+  </si>
+  <si>
+    <t>Fuel Flow (GPH)</t>
+  </si>
+  <si>
+    <t>True Airspeed (Knots)</t>
+  </si>
+  <si>
+    <t>Diff. Fuel Flow</t>
+  </si>
+  <si>
+    <t>Diff. True Airspeed</t>
+  </si>
+  <si>
+    <t>Diff. Range</t>
+  </si>
+  <si>
+    <t>Range (Nautical Miles)</t>
   </si>
 </sst>
 </file>
@@ -96,9 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2726,7 +2746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49353E1-1EC1-5A40-9077-1E137B7BE37E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2953,4 +2973,120 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0005834-5C08-2248-90F6-10108CA4B04C}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <f>(72/B2)*C2</f>
+        <v>774.19354838709671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>10.9</v>
+      </c>
+      <c r="C3">
+        <v>115</v>
+      </c>
+      <c r="D3" s="2">
+        <f>(72/B3)*C3</f>
+        <v>759.63302752293566</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(B3-B2)/B2</f>
+        <v>0.17204301075268813</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(C3-C2)/C2</f>
+        <v>0.15</v>
+      </c>
+      <c r="G3" s="1">
+        <f>(D3-D2)/D2</f>
+        <v>-1.8807339449541355E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>12.65</v>
+      </c>
+      <c r="C4">
+        <v>124</v>
+      </c>
+      <c r="D4" s="2">
+        <f>(72/B4)*C4</f>
+        <v>705.77075098814225</v>
+      </c>
+      <c r="E4" s="1">
+        <f>(B4-B3)/B3</f>
+        <v>0.16055045871559631</v>
+      </c>
+      <c r="F4" s="1">
+        <f>(C4-C3)/C3</f>
+        <v>7.8260869565217397E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <f>(D4-D3)/D3</f>
+        <v>-7.0905653892421289E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add fuel flow comparison for 50F ROP
</commit_message>
<xml_diff>
--- a/pa-28-236/pa-28-236.xlsx
+++ b/pa-28-236/pa-28-236.xlsx
@@ -8,16 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-28-236/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D6E4D2-9F6E-FE41-8D24-57B0EF22A6E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73283888-2FC7-4E4A-A579-26A4C23E9BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3060" windowWidth="37760" windowHeight="19340" activeTab="3" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
+    <workbookView xWindow="2500" yWindow="1080" windowWidth="37760" windowHeight="19340" activeTab="4" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
   </bookViews>
   <sheets>
     <sheet name="KIAS Vs. % Power (50F ROP)" sheetId="1" r:id="rId1"/>
     <sheet name="KIAS Vs. % Power (Peak EGT)" sheetId="3" r:id="rId2"/>
     <sheet name="Altitude Vs. IAS at 65% (Eco)" sheetId="4" r:id="rId3"/>
-    <sheet name="Fuel Flow Comparison" sheetId="5" r:id="rId4"/>
+    <sheet name="Fuel Flow Comparison (Peak EGT)" sheetId="5" r:id="rId4"/>
+    <sheet name="Fuel Flow Comparison (50F ROP)" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$1:$G$1</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$2:$G$2</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$3:$G$3</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$4:$G$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Percent Power</t>
   </si>
@@ -2669,7 +2676,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2979,19 +2986,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0005834-5C08-2248-90F6-10108CA4B04C}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3089,4 +3096,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE9ACF9-1AAF-A640-8D8F-D305269B4D67}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>10.1</v>
+      </c>
+      <c r="C2">
+        <v>104</v>
+      </c>
+      <c r="D2" s="2">
+        <f>(72/B2)*C2</f>
+        <v>741.38613861386136</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>11.8</v>
+      </c>
+      <c r="C3">
+        <v>117</v>
+      </c>
+      <c r="D3" s="2">
+        <f>(72/B3)*C3</f>
+        <v>713.89830508474574</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(B3-B2)/B2</f>
+        <v>0.16831683168316844</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(C3-C2)/C2</f>
+        <v>0.125</v>
+      </c>
+      <c r="G3" s="1">
+        <f>(D3-D2)/D2</f>
+        <v>-3.7076271186440676E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>13.6</v>
+      </c>
+      <c r="C4">
+        <v>126</v>
+      </c>
+      <c r="D4" s="2">
+        <f>(72/B4)*C4</f>
+        <v>667.05882352941171</v>
+      </c>
+      <c r="E4" s="1">
+        <f>(B4-B3)/B3</f>
+        <v>0.15254237288135583</v>
+      </c>
+      <c r="F4" s="1">
+        <f>(C4-C3)/C3</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <f>(D4-D3)/D3</f>
+        <v>-6.5610859728506832E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>85</v>
+      </c>
+      <c r="B5">
+        <v>15.2</v>
+      </c>
+      <c r="C5">
+        <v>134</v>
+      </c>
+      <c r="D5" s="2">
+        <f>(72/B5)*C5</f>
+        <v>634.73684210526324</v>
+      </c>
+      <c r="E5" s="1">
+        <f>(B5-B4)/B4</f>
+        <v>0.11764705882352938</v>
+      </c>
+      <c r="F5" s="1">
+        <f>(C5-C4)/C4</f>
+        <v>6.3492063492063489E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <f>(D5-D4)/D4</f>
+        <v>-4.8454469507100896E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PA-28-236: Add Weight Vs. Maneuvering Speed
In addition, begin comparison of percent power to fuel flow, TAS, and range.
</commit_message>
<xml_diff>
--- a/pa-28-236/pa-28-236.xlsx
+++ b/pa-28-236/pa-28-236.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-28-236/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73283888-2FC7-4E4A-A579-26A4C23E9BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172A46BD-04B9-8044-A2F4-84EDD85DC45F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1080" windowWidth="37760" windowHeight="19340" activeTab="4" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
+    <workbookView xWindow="640" yWindow="980" windowWidth="37760" windowHeight="19340" activeTab="5" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
   </bookViews>
   <sheets>
     <sheet name="KIAS Vs. % Power (50F ROP)" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,8 @@
     <sheet name="Altitude Vs. IAS at 65% (Eco)" sheetId="4" r:id="rId3"/>
     <sheet name="Fuel Flow Comparison (Peak EGT)" sheetId="5" r:id="rId4"/>
     <sheet name="Fuel Flow Comparison (50F ROP)" sheetId="6" r:id="rId5"/>
+    <sheet name="Weight Vs. Maneuvering Speed" sheetId="7" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$1:$G$1</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$2:$G$2</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$3:$G$3</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Fuel Flow Comparison (Peak EGT)'!$A$4:$G$4</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Percent Power</t>
   </si>
@@ -79,6 +74,12 @@
   </si>
   <si>
     <t>Range (Nautical Miles)</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Maneuvering Speed</t>
   </si>
 </sst>
 </file>
@@ -1420,6 +1421,1486 @@
   </c:printSettings>
   <c:userShapes r:id="rId2"/>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>True Airspeed (Knots)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>134</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C946-5747-8224-74FF27499DD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="525594432"/>
+        <c:axId val="525749344"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fuel Flow (GPH)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41EE-2B45-A911-3CCA289D669A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Range (Nautical Miles)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fuel Flow Comparison (50F ROP)'!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>741.38613861386136</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>713.89830508474574</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>667.05882352941171</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>634.73684210526324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C946-5747-8224-74FF27499DD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="525605344"/>
+        <c:axId val="475864304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="525594432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525749344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="525749344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525594432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="475864304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="600"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525605344"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="525605344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="475864304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Weight</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Vs. Maneuvering Speed</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8306453225946247E-2"/>
+          <c:y val="0.19618456294903228"/>
+          <c:w val="0.91603312287064875"/>
+          <c:h val="0.77220754326797125"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Weight Vs. Maneuvering Speed'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Maneuvering Speed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0">
+                      <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                      <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Weight Vs. Maneuvering Speed'!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1761</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Weight Vs. Maneuvering Speed'!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-917B-8345-9694-A78B60768DB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="951141263"/>
+        <c:axId val="948993503"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="951141263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3100"/>
+          <c:min val="1700"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="948993503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="200"/>
+        <c:minorUnit val="100"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="948993503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="130"/>
+          <c:min val="90"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="951141263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1802,6 +3283,90 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>850900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>130810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23AA08D6-7953-964C-B119-0BD420014246}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>694267</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>70812</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>56782</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37CEFB3B-3839-D947-BDDA-3EDCD0B324D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2671,12 +4236,298 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147924CF-2EF1-8C42-B7BB-87C12FB00719}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2804,6 +4655,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3054,15 +4906,15 @@
         <v>759.63302752293566</v>
       </c>
       <c r="E3" s="1">
-        <f>(B3-B2)/B2</f>
+        <f t="shared" ref="E3:G4" si="0">(B3-B2)/B2</f>
         <v>0.17204301075268813</v>
       </c>
       <c r="F3" s="1">
-        <f>(C3-C2)/C2</f>
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
       <c r="G3" s="1">
-        <f>(D3-D2)/D2</f>
+        <f t="shared" si="0"/>
         <v>-1.8807339449541355E-2</v>
       </c>
     </row>
@@ -3081,20 +4933,21 @@
         <v>705.77075098814225</v>
       </c>
       <c r="E4" s="1">
-        <f>(B4-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>0.16055045871559631</v>
       </c>
       <c r="F4" s="1">
-        <f>(C4-C3)/C3</f>
+        <f t="shared" si="0"/>
         <v>7.8260869565217397E-2</v>
       </c>
       <c r="G4" s="1">
-        <f>(D4-D3)/D3</f>
+        <f t="shared" si="0"/>
         <v>-7.0905653892421289E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3102,8 +4955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE9ACF9-1AAF-A640-8D8F-D305269B4D67}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3171,15 +5024,15 @@
         <v>713.89830508474574</v>
       </c>
       <c r="E3" s="1">
-        <f>(B3-B2)/B2</f>
+        <f t="shared" ref="E3:G5" si="0">(B3-B2)/B2</f>
         <v>0.16831683168316844</v>
       </c>
       <c r="F3" s="1">
-        <f>(C3-C2)/C2</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="G3" s="1">
-        <f>(D3-D2)/D2</f>
+        <f t="shared" si="0"/>
         <v>-3.7076271186440676E-2</v>
       </c>
     </row>
@@ -3198,15 +5051,15 @@
         <v>667.05882352941171</v>
       </c>
       <c r="E4" s="1">
-        <f>(B4-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>0.15254237288135583</v>
       </c>
       <c r="F4" s="1">
-        <f>(C4-C3)/C3</f>
+        <f t="shared" si="0"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="G4" s="1">
-        <f>(D4-D3)/D3</f>
+        <f t="shared" si="0"/>
         <v>-6.5610859728506832E-2</v>
       </c>
     </row>
@@ -3225,15 +5078,15 @@
         <v>634.73684210526324</v>
       </c>
       <c r="E5" s="1">
-        <f>(B5-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>0.11764705882352938</v>
       </c>
       <c r="F5" s="1">
-        <f>(C5-C4)/C4</f>
+        <f t="shared" si="0"/>
         <v>6.3492063492063489E-2</v>
       </c>
       <c r="G5" s="1">
-        <f>(D5-D4)/D4</f>
+        <f t="shared" si="0"/>
         <v>-4.8454469507100896E-2</v>
       </c>
     </row>
@@ -3254,5 +5107,51 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86E6CB7-33FF-D845-BEFE-836C7083FECD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3000</v>
+      </c>
+      <c r="B2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1761</v>
+      </c>
+      <c r="B3">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PA-28-236: Indicated → Calibrated Airspeed
</commit_message>
<xml_diff>
--- a/pa-28-236/pa-28-236.xlsx
+++ b/pa-28-236/pa-28-236.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-28-236/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172A46BD-04B9-8044-A2F4-84EDD85DC45F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9AD48E-AECE-AD4A-B372-215344361A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="980" windowWidth="37760" windowHeight="19340" activeTab="5" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
+    <workbookView xWindow="640" yWindow="980" windowWidth="37760" windowHeight="19340" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
   </bookViews>
   <sheets>
-    <sheet name="KIAS Vs. % Power (50F ROP)" sheetId="1" r:id="rId1"/>
-    <sheet name="KIAS Vs. % Power (Peak EGT)" sheetId="3" r:id="rId2"/>
-    <sheet name="Altitude Vs. IAS at 65% (Eco)" sheetId="4" r:id="rId3"/>
+    <sheet name="KCAS Vs. % Power (50F ROP)" sheetId="1" r:id="rId1"/>
+    <sheet name="KCAS Vs. % Power (Peak EGT)" sheetId="3" r:id="rId2"/>
+    <sheet name="Altitude Vs. KCAS at 65% (Eco)" sheetId="4" r:id="rId3"/>
     <sheet name="Fuel Flow Comparison (Peak EGT)" sheetId="5" r:id="rId4"/>
     <sheet name="Fuel Flow Comparison (50F ROP)" sheetId="6" r:id="rId5"/>
     <sheet name="Weight Vs. Maneuvering Speed" sheetId="7" r:id="rId6"/>
@@ -43,16 +43,7 @@
     <t>Percent Power</t>
   </si>
   <si>
-    <t>KIAS (50°F ROP)</t>
-  </si>
-  <si>
-    <t>KIAS (Peak EGT)</t>
-  </si>
-  <si>
     <t>Pressure Altitude</t>
-  </si>
-  <si>
-    <t>KIAS</t>
   </si>
   <si>
     <t>KTAS</t>
@@ -80,6 +71,15 @@
   </si>
   <si>
     <t>Maneuvering Speed</t>
+  </si>
+  <si>
+    <t>KCAS (50°F ROP)</t>
+  </si>
+  <si>
+    <t>KCAS</t>
+  </si>
+  <si>
+    <t>KCAS (Peak EGT)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Indicated Airspeed Vs. Percent Power</a:t>
+              <a:t>Calibrated Airspeed Vs. Percent Power</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -285,11 +285,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KIAS Vs. % Power (50F ROP)'!$B$1</c:f>
+              <c:f>'KCAS Vs. % Power (50F ROP)'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KIAS (50°F ROP)</c:v>
+                  <c:v>KCAS (50°F ROP)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -328,7 +328,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'KIAS Vs. % Power (50F ROP)'!$A$2:$A$7</c:f>
+              <c:f>'KCAS Vs. % Power (50F ROP)'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -352,7 +352,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'KIAS Vs. % Power (50F ROP)'!$B$2:$B$7</c:f>
+              <c:f>'KCAS Vs. % Power (50F ROP)'!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -610,7 +610,7 @@
                 <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
                 <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
               </a:rPr>
-              <a:t>Indicated</a:t>
+              <a:t>Calibrated</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
@@ -729,11 +729,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KIAS Vs. % Power (Peak EGT)'!$B$1</c:f>
+              <c:f>'KCAS Vs. % Power (Peak EGT)'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KIAS (Peak EGT)</c:v>
+                  <c:v>KCAS (Peak EGT)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -773,7 +773,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'KIAS Vs. % Power (Peak EGT)'!$A$2:$A$4</c:f>
+              <c:f>'KCAS Vs. % Power (Peak EGT)'!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -791,7 +791,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'KIAS Vs. % Power (Peak EGT)'!$B$2:$B$4</c:f>
+              <c:f>'KCAS Vs. % Power (Peak EGT)'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1042,7 +1042,7 @@
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Pressure Altitude Vs. Indicated Airspeed</a:t>
+              <a:t>Pressure Altitude Vs. Calibrated Airspeed</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="en-US"/>
@@ -1087,11 +1087,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Altitude Vs. IAS at 65% (Eco)'!$B$1</c:f>
+              <c:f>'Altitude Vs. KCAS at 65% (Eco)'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KIAS</c:v>
+                  <c:v>KCAS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1164,7 +1164,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Altitude Vs. IAS at 65% (Eco)'!$A$2:$A$14</c:f>
+              <c:f>'Altitude Vs. KCAS at 65% (Eco)'!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1212,7 +1212,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Altitude Vs. IAS at 65% (Eco)'!$B$2:$B$14</c:f>
+              <c:f>'Altitude Vs. KCAS at 65% (Eco)'!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4526,8 +4526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147924CF-2EF1-8C42-B7BB-87C12FB00719}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4542,7 +4542,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4605,7 +4605,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4620,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4665,7 +4665,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4675,13 +4675,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4858,22 +4858,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -4975,22 +4975,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -5116,8 +5116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86E6CB7-33FF-D845-BEFE-836C7083FECD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5127,10 +5127,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>